<commit_message>
Correção definitiva do relatório de lucratividade por item
</commit_message>
<xml_diff>
--- a/modelo_lucro_item.xlsx
+++ b/modelo_lucro_item.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuário\wesll\PycharmProjects\meu_preco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9010\PycharmProjects\meu_preco1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A07AEC-44CE-473F-9A4C-DC9E22E7CDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C699EFD-0332-4D99-BCAF-0AF318528635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F2B51D2-9080-4D45-881D-AE3C33C2FF7A}"/>
   </bookViews>
@@ -136,11 +136,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,10 +170,17 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,7 +495,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +509,8 @@
     <col min="7" max="7" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="10" max="10" width="9.140625" style="11"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -532,7 +541,7 @@
       <c r="I1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizacao da query de despesa
</commit_message>
<xml_diff>
--- a/modelo_lucro_item.xlsx
+++ b/modelo_lucro_item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9010\PycharmProjects\meu_preco1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C699EFD-0332-4D99-BCAF-0AF318528635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4029F71-5D20-461E-A24A-AE3A18BF02DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6F2B51D2-9080-4D45-881D-AE3C33C2FF7A}"/>
   </bookViews>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -141,7 +140,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -164,10 +163,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -175,6 +174,18 @@
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -495,7 +506,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,11 +514,11 @@
     <col min="1" max="1" width="6.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="9" style="5" customWidth="1"/>
     <col min="3" max="3" width="9" style="7" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" style="9" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="9" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="11"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
@@ -523,7 +534,7 @@
       <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
@@ -535,7 +546,7 @@
       <c r="G1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="8" t="s">

</xml_diff>